<commit_message>
integrated w sqlite fully
</commit_message>
<xml_diff>
--- a/static/Chinese Vocab Community.xlsx
+++ b/static/Chinese Vocab Community.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="ep 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="osu! writeup" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="1132">
   <si>
     <t>Characters</t>
   </si>
@@ -2134,6 +2135,12 @@
     <t>note, inject</t>
   </si>
   <si>
+    <t>注册</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
     <t>意</t>
   </si>
   <si>
@@ -2348,6 +2355,1059 @@
   </si>
   <si>
     <t>easy going</t>
+  </si>
+  <si>
+    <t>当</t>
+  </si>
+  <si>
+    <t>dāng</t>
+  </si>
+  <si>
+    <t>equal, work as, manage</t>
+  </si>
+  <si>
+    <t>当然</t>
+  </si>
+  <si>
+    <t>dāngrán</t>
+  </si>
+  <si>
+    <t>certainly</t>
+  </si>
+  <si>
+    <t>邀</t>
+  </si>
+  <si>
+    <t>yāo</t>
+  </si>
+  <si>
+    <t>invite</t>
+  </si>
+  <si>
+    <t>出</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chū		</t>
+  </si>
+  <si>
+    <t>come out, put out</t>
+  </si>
+  <si>
+    <t>任何</t>
+  </si>
+  <si>
+    <t>rènhé</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>由来</t>
+  </si>
+  <si>
+    <t>yóulái</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>给</t>
+  </si>
+  <si>
+    <t>gěi</t>
+  </si>
+  <si>
+    <t>give</t>
+  </si>
+  <si>
+    <t>联系</t>
+  </si>
+  <si>
+    <t>liánxì</t>
+  </si>
+  <si>
+    <t>connect</t>
+  </si>
+  <si>
+    <t>酷</t>
+  </si>
+  <si>
+    <t>kù</t>
+  </si>
+  <si>
+    <t>cool (not temp)</t>
+  </si>
+  <si>
+    <t>像</t>
+  </si>
+  <si>
+    <t>similar</t>
+  </si>
+  <si>
+    <t>电影</t>
+  </si>
+  <si>
+    <t>diànyǐng</t>
+  </si>
+  <si>
+    <t>movie</t>
+  </si>
+  <si>
+    <t>餐</t>
+  </si>
+  <si>
+    <t>cān</t>
+  </si>
+  <si>
+    <t>meal</t>
+  </si>
+  <si>
+    <t>俱</t>
+  </si>
+  <si>
+    <t>jù</t>
+  </si>
+  <si>
+    <t>俱乐部</t>
+  </si>
+  <si>
+    <t>jùlèbù</t>
+  </si>
+  <si>
+    <t>club</t>
+  </si>
+  <si>
+    <t>相</t>
+  </si>
+  <si>
+    <t>xiāng</t>
+  </si>
+  <si>
+    <t>mutually, picture</t>
+  </si>
+  <si>
+    <t>相信</t>
+  </si>
+  <si>
+    <t>xiāngxìn</t>
+  </si>
+  <si>
+    <t>trust</t>
+  </si>
+  <si>
+    <t>相对</t>
+  </si>
+  <si>
+    <t>xiāngduì</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>憋</t>
+  </si>
+  <si>
+    <t>biē</t>
+  </si>
+  <si>
+    <t>supress, oppress</t>
+  </si>
+  <si>
+    <t>肚子</t>
+  </si>
+  <si>
+    <t>dùzi</t>
+  </si>
+  <si>
+    <t>stomach</t>
+  </si>
+  <si>
+    <t>烦心</t>
+  </si>
+  <si>
+    <t>fánxīn</t>
+  </si>
+  <si>
+    <t>痛哭</t>
+  </si>
+  <si>
+    <t>tòngkū</t>
+  </si>
+  <si>
+    <t>cry</t>
+  </si>
+  <si>
+    <t>伙</t>
+  </si>
+  <si>
+    <t>huǒ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partner </t>
+  </si>
+  <si>
+    <t>大伙</t>
+  </si>
+  <si>
+    <t>everyone</t>
+  </si>
+  <si>
+    <t>绪</t>
+  </si>
+  <si>
+    <t>xù</t>
+  </si>
+  <si>
+    <t>thread, clue</t>
+  </si>
+  <si>
+    <t>情绪</t>
+  </si>
+  <si>
+    <t>mood</t>
+  </si>
+  <si>
+    <t>腔</t>
+  </si>
+  <si>
+    <t>qiāng</t>
+  </si>
+  <si>
+    <t>cavity, accent</t>
+  </si>
+  <si>
+    <t>短</t>
+  </si>
+  <si>
+    <t>duǎn</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>读</t>
+  </si>
+  <si>
+    <t>dú</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>家伙</t>
+  </si>
+  <si>
+    <t>jiāhuǒ</t>
+  </si>
+  <si>
+    <t>guy (casual)</t>
+  </si>
+  <si>
+    <t>尿（尿）</t>
+  </si>
+  <si>
+    <t>niào</t>
+  </si>
+  <si>
+    <t>pee</t>
+  </si>
+  <si>
+    <t>奇怪</t>
+  </si>
+  <si>
+    <t>qíguài</t>
+  </si>
+  <si>
+    <t>strange</t>
+  </si>
+  <si>
+    <t>住</t>
+  </si>
+  <si>
+    <t>live</t>
+  </si>
+  <si>
+    <t>难住</t>
+  </si>
+  <si>
+    <t>stumped</t>
+  </si>
+  <si>
+    <t>确</t>
+  </si>
+  <si>
+    <t>què</t>
+  </si>
+  <si>
+    <t>correct, indeed</t>
+  </si>
+  <si>
+    <t>橄榄球</t>
+  </si>
+  <si>
+    <t>gǎnlǎnqiú</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chǎng	</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>缩</t>
+  </si>
+  <si>
+    <t>suō</t>
+  </si>
+  <si>
+    <t>shrink</t>
+  </si>
+  <si>
+    <t>钟</t>
+  </si>
+  <si>
+    <t>zhōng</t>
+  </si>
+  <si>
+    <t>bell</t>
+  </si>
+  <si>
+    <t>分钟</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>继续</t>
+  </si>
+  <si>
+    <t>jìxù</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>动</t>
+  </si>
+  <si>
+    <t>dòng</t>
+  </si>
+  <si>
+    <t>move</t>
+  </si>
+  <si>
+    <t>词</t>
+  </si>
+  <si>
+    <t>cí</t>
+  </si>
+  <si>
+    <t>假</t>
+  </si>
+  <si>
+    <t>jiǎ</t>
+  </si>
+  <si>
+    <t>fake</t>
+  </si>
+  <si>
+    <t>弄</t>
+  </si>
+  <si>
+    <t>nòng</t>
+  </si>
+  <si>
+    <t>alley, fetch</t>
+  </si>
+  <si>
+    <t>辨</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biàn		</t>
+  </si>
+  <si>
+    <t>distinguish</t>
+  </si>
+  <si>
+    <t>幼</t>
+  </si>
+  <si>
+    <t>young</t>
+  </si>
+  <si>
+    <t>混淆</t>
+  </si>
+  <si>
+    <t>hùnxiáo</t>
+  </si>
+  <si>
+    <t>confuse</t>
+  </si>
+  <si>
+    <t>要么</t>
+  </si>
+  <si>
+    <t>yàome</t>
+  </si>
+  <si>
+    <t>either</t>
+  </si>
+  <si>
+    <t>论</t>
+  </si>
+  <si>
+    <t>lùn</t>
+  </si>
+  <si>
+    <t>argument</t>
+  </si>
+  <si>
+    <t>不论</t>
+  </si>
+  <si>
+    <t>bǔlùn</t>
+  </si>
+  <si>
+    <t>whether, regardless</t>
+  </si>
+  <si>
+    <t>发生</t>
+  </si>
+  <si>
+    <t>fāshēng</t>
+  </si>
+  <si>
+    <t>occur</t>
+  </si>
+  <si>
+    <t>常</t>
+  </si>
+  <si>
+    <t>cháng</t>
+  </si>
+  <si>
+    <t>often</t>
+  </si>
+  <si>
+    <t>正常</t>
+  </si>
+  <si>
+    <t>zhèngcháng</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>道德</t>
+  </si>
+  <si>
+    <t>dàodé</t>
+  </si>
+  <si>
+    <t>morals</t>
+  </si>
+  <si>
+    <t>脱</t>
+  </si>
+  <si>
+    <t>tuō</t>
+  </si>
+  <si>
+    <t>come off, take off</t>
+  </si>
+  <si>
+    <t>脱口而出</t>
+  </si>
+  <si>
+    <t>blurt out</t>
+  </si>
+  <si>
+    <t>口</t>
+  </si>
+  <si>
+    <t>kǒu</t>
+  </si>
+  <si>
+    <t>mouth, opening</t>
+  </si>
+  <si>
+    <t>扮</t>
+  </si>
+  <si>
+    <t>bàn</t>
+  </si>
+  <si>
+    <t>pretend</t>
+  </si>
+  <si>
+    <t>心里</t>
+  </si>
+  <si>
+    <t>xīnlǐ</t>
+  </si>
+  <si>
+    <t>psychology</t>
+  </si>
+  <si>
+    <t>医生</t>
+  </si>
+  <si>
+    <t>yīshēng</t>
+  </si>
+  <si>
+    <t>doctor</t>
+  </si>
+  <si>
+    <t>卫</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wèi	</t>
+  </si>
+  <si>
+    <t>defend</t>
+  </si>
+  <si>
+    <t>尊</t>
+  </si>
+  <si>
+    <t>zūn</t>
+  </si>
+  <si>
+    <t>respect</t>
+  </si>
+  <si>
+    <t>接受</t>
+  </si>
+  <si>
+    <t>jiēshòu</t>
+  </si>
+  <si>
+    <t>accept</t>
+  </si>
+  <si>
+    <t>事实</t>
+  </si>
+  <si>
+    <t>shìshí</t>
+  </si>
+  <si>
+    <t>fact</t>
+  </si>
+  <si>
+    <t>胆</t>
+  </si>
+  <si>
+    <t>dǎn</t>
+  </si>
+  <si>
+    <t>courage</t>
+  </si>
+  <si>
+    <t>胆小鬼</t>
+  </si>
+  <si>
+    <t>coward</t>
+  </si>
+  <si>
+    <t>鬼</t>
+  </si>
+  <si>
+    <t>guǐ</t>
+  </si>
+  <si>
+    <t>ghost, sinister</t>
+  </si>
+  <si>
+    <t>授</t>
+  </si>
+  <si>
+    <t>shòu</t>
+  </si>
+  <si>
+    <t>teach</t>
+  </si>
+  <si>
+    <t>姑</t>
+  </si>
+  <si>
+    <t>gū</t>
+  </si>
+  <si>
+    <t>aunt (paternal side)</t>
+  </si>
+  <si>
+    <t>娘</t>
+  </si>
+  <si>
+    <t>niǎng</t>
+  </si>
+  <si>
+    <t>mother</t>
+  </si>
+  <si>
+    <t>姑娘</t>
+  </si>
+  <si>
+    <t>gūniǎng</t>
+  </si>
+  <si>
+    <t>girl</t>
+  </si>
+  <si>
+    <t>形</t>
+  </si>
+  <si>
+    <t>xíng</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>吼</t>
+  </si>
+  <si>
+    <t>hǒu</t>
+  </si>
+  <si>
+    <t>yell</t>
+  </si>
+  <si>
+    <t>客</t>
+  </si>
+  <si>
+    <t>kè</t>
+  </si>
+  <si>
+    <t>guest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">客气	</t>
+  </si>
+  <si>
+    <t>polite</t>
+  </si>
+  <si>
+    <t>嘴</t>
+  </si>
+  <si>
+    <t>zuǐ</t>
+  </si>
+  <si>
+    <t>mouth</t>
+  </si>
+  <si>
+    <t>结</t>
+  </si>
+  <si>
+    <t>jié</t>
+  </si>
+  <si>
+    <t>knot</t>
+  </si>
+  <si>
+    <t>束</t>
+  </si>
+  <si>
+    <t>bundle</t>
+  </si>
+  <si>
+    <t>结束</t>
+  </si>
+  <si>
+    <t>jiéshù</t>
+  </si>
+  <si>
+    <t>finish</t>
+  </si>
+  <si>
+    <t>临时</t>
+  </si>
+  <si>
+    <t>línshí</t>
+  </si>
+  <si>
+    <t>temporary</t>
+  </si>
+  <si>
+    <t>保</t>
+  </si>
+  <si>
+    <t>save protect</t>
+  </si>
+  <si>
+    <t>保姆</t>
+  </si>
+  <si>
+    <t>bǎomǔ</t>
+  </si>
+  <si>
+    <t>baby sit</t>
+  </si>
+  <si>
+    <t>颁</t>
+  </si>
+  <si>
+    <t>issue, award</t>
+  </si>
+  <si>
+    <t>从</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cóng	</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>棒</t>
+  </si>
+  <si>
+    <t>bàng</t>
+  </si>
+  <si>
+    <t>great</t>
+  </si>
+  <si>
+    <t>棒得没法</t>
+  </si>
+  <si>
+    <t>too good to be true</t>
+  </si>
+  <si>
+    <t>几</t>
+  </si>
+  <si>
+    <t>jǐ</t>
+  </si>
+  <si>
+    <t>several</t>
+  </si>
+  <si>
+    <t>洗</t>
+  </si>
+  <si>
+    <t>xǐ</t>
+  </si>
+  <si>
+    <t>wash</t>
+  </si>
+  <si>
+    <t>间</t>
+  </si>
+  <si>
+    <t>jiān</t>
+  </si>
+  <si>
+    <t>between</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinese </t>
+  </si>
+  <si>
+    <t>Def</t>
+  </si>
+  <si>
+    <t>should have known</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read </t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>取</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qǔ	</t>
+  </si>
+  <si>
+    <t>pick, take</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>档</t>
+  </si>
+  <si>
+    <t>dàng</t>
+  </si>
+  <si>
+    <t>files, pigeonhole</t>
+  </si>
+  <si>
+    <t>案</t>
+  </si>
+  <si>
+    <t>àn</t>
+  </si>
+  <si>
+    <t>case, proposal, file</t>
+  </si>
+  <si>
+    <t>谱</t>
+  </si>
+  <si>
+    <t>pǔ</t>
+  </si>
+  <si>
+    <t>music, list, spectrum</t>
+  </si>
+  <si>
+    <t>面</t>
+  </si>
+  <si>
+    <t>miàn</t>
+  </si>
+  <si>
+    <t>noodle, external</t>
+  </si>
+  <si>
+    <t>谱面</t>
+  </si>
+  <si>
+    <t>pǔmiàn</t>
+  </si>
+  <si>
+    <t>chart</t>
+  </si>
+  <si>
+    <t>记录</t>
+  </si>
+  <si>
+    <t>jìlù</t>
+  </si>
+  <si>
+    <t>record</t>
+  </si>
+  <si>
+    <t>计算</t>
+  </si>
+  <si>
+    <t>jìsuàn</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>标</t>
+  </si>
+  <si>
+    <t>biāo</t>
+  </si>
+  <si>
+    <t>mark</t>
+  </si>
+  <si>
+    <t>目标</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>排</t>
+  </si>
+  <si>
+    <t>pái</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>排行</t>
+  </si>
+  <si>
+    <t>páiháng</t>
+  </si>
+  <si>
+    <t>ranking</t>
+  </si>
+  <si>
+    <t>榜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bǎng	</t>
+  </si>
+  <si>
+    <t>list, notice</t>
+  </si>
+  <si>
+    <t>拿</t>
+  </si>
+  <si>
+    <t>ná</t>
+  </si>
+  <si>
+    <t>take</t>
+  </si>
+  <si>
+    <t>not fucking 事</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quiet </t>
+  </si>
+  <si>
+    <t>态</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tài		</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>静态</t>
+  </si>
+  <si>
+    <t>jìngtài</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>低</t>
+  </si>
+  <si>
+    <t>dī</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>脚</t>
+  </si>
+  <si>
+    <t>jiǎo</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>脚本</t>
+  </si>
+  <si>
+    <t>jiǎoběn</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>改</t>
+  </si>
+  <si>
+    <t>gǎi</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>改写</t>
+  </si>
+  <si>
+    <t>gǎixiě</t>
+  </si>
+  <si>
+    <t>rewrite</t>
+  </si>
+  <si>
+    <t>能过</t>
+  </si>
+  <si>
+    <t>néngguò</t>
+  </si>
+  <si>
+    <t>can pass</t>
+  </si>
+  <si>
+    <t>边</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biān	</t>
+  </si>
+  <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>配</t>
+  </si>
+  <si>
+    <t>pèi</t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>随</t>
+  </si>
+  <si>
+    <t>suí</t>
+  </si>
+  <si>
+    <t>follow, adapt</t>
+  </si>
+  <si>
+    <t>随便</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suíbiàn	</t>
+  </si>
+  <si>
+    <t>casual, feel free to, etc</t>
+  </si>
+  <si>
+    <t>爆炸</t>
+  </si>
+  <si>
+    <t>bàozhà</t>
+  </si>
+  <si>
+    <t>explode, blow out</t>
+  </si>
+  <si>
+    <t>方法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fāngfǎ		</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>不过</t>
+  </si>
+  <si>
+    <t>bùguò</t>
+  </si>
+  <si>
+    <t xml:space="preserve">but </t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>帐</t>
+  </si>
+  <si>
+    <t>zhàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">account, tent </t>
+  </si>
+  <si>
+    <t>号</t>
+  </si>
+  <si>
+    <t>hào</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number </t>
   </si>
 </sst>
 </file>
@@ -2397,6 +3457,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -5222,58 +6286,64 @@
       <c r="C219" s="1" t="s">
         <v>706</v>
       </c>
+      <c r="D219" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>251</v>
@@ -5281,82 +6351,82 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>327</v>
@@ -5364,38 +6434,38 @@
     </row>
     <row r="231">
       <c r="A231" s="1" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>600</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>330</v>
@@ -5403,101 +6473,1531 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>778</v>
+        <v>780</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="E310" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added database update script and usage stats (not readable from web app yet)
</commit_message>
<xml_diff>
--- a/static/Chinese Vocab Community.xlsx
+++ b/static/Chinese Vocab Community.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ep 1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="osu! writeup" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sheet3" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="osu! writeup" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="1132">
   <si>
     <t>Characters</t>
   </si>
@@ -3461,6 +3462,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -7526,6 +7531,187 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>1031</v>
       </c>
       <c r="B1" s="1" t="s">

</xml_diff>

<commit_message>
updated xlsx, should be last one
</commit_message>
<xml_diff>
--- a/static/Chinese Vocab Community.xlsx
+++ b/static/Chinese Vocab Community.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="1547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="1975">
   <si>
     <t>Characters</t>
   </si>
@@ -2237,7 +2237,7 @@
     <t>情况</t>
   </si>
   <si>
-    <t>qíngjuàng</t>
+    <t>qíngkuàng</t>
   </si>
   <si>
     <t>situation</t>
@@ -4367,6 +4367,1311 @@
     <t>graduate</t>
   </si>
   <si>
+    <t>舞</t>
+  </si>
+  <si>
+    <t>wǔ</t>
+  </si>
+  <si>
+    <t>dance</t>
+  </si>
+  <si>
+    <t>国王</t>
+  </si>
+  <si>
+    <t>guówáng</t>
+  </si>
+  <si>
+    <t>king</t>
+  </si>
+  <si>
+    <t>河</t>
+  </si>
+  <si>
+    <t>river</t>
+  </si>
+  <si>
+    <t>畔</t>
+  </si>
+  <si>
+    <t>pàn</t>
+  </si>
+  <si>
+    <t>beside</t>
+  </si>
+  <si>
+    <t>高中</t>
+  </si>
+  <si>
+    <t>gāozhōng</t>
+  </si>
+  <si>
+    <t>highschool</t>
+  </si>
+  <si>
+    <t>穿</t>
+  </si>
+  <si>
+    <t>chuān</t>
+  </si>
+  <si>
+    <t>wear</t>
+  </si>
+  <si>
+    <t>愚蠢</t>
+  </si>
+  <si>
+    <t>yúchǔn</t>
+  </si>
+  <si>
+    <t>stupid</t>
+  </si>
+  <si>
+    <t>母</t>
+  </si>
+  <si>
+    <t>mǔ</t>
+  </si>
+  <si>
+    <t>字母</t>
+  </si>
+  <si>
+    <t>zimǔ</t>
+  </si>
+  <si>
+    <t>letters</t>
+  </si>
+  <si>
+    <t>药</t>
+  </si>
+  <si>
+    <t>yào</t>
+  </si>
+  <si>
+    <t>drugs, medicine</t>
+  </si>
+  <si>
+    <t>嗑药（嗑）</t>
+  </si>
+  <si>
+    <t>kēyàokē</t>
+  </si>
+  <si>
+    <t>take drugs</t>
+  </si>
+  <si>
+    <t>药丸</t>
+  </si>
+  <si>
+    <t>yàowán</t>
+  </si>
+  <si>
+    <t>pill</t>
+  </si>
+  <si>
+    <t>退</t>
+  </si>
+  <si>
+    <t>tuì</t>
+  </si>
+  <si>
+    <t>retreat, withdraw</t>
+  </si>
+  <si>
+    <t>远动</t>
+  </si>
+  <si>
+    <t>yuǎndòng</t>
+  </si>
+  <si>
+    <t>sports</t>
+  </si>
+  <si>
+    <t>蛋</t>
+  </si>
+  <si>
+    <t>dàn</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>傻</t>
+  </si>
+  <si>
+    <t>shǎ</t>
+  </si>
+  <si>
+    <t>傻蛋</t>
+  </si>
+  <si>
+    <t>shǎdàn</t>
+  </si>
+  <si>
+    <t>idiot (egghead)</t>
+  </si>
+  <si>
+    <t>倒</t>
+  </si>
+  <si>
+    <t>dào</t>
+  </si>
+  <si>
+    <t>fall</t>
+  </si>
+  <si>
+    <t>立</t>
+  </si>
+  <si>
+    <t>lì</t>
+  </si>
+  <si>
+    <t>stand</t>
+  </si>
+  <si>
+    <t>倒立</t>
+  </si>
+  <si>
+    <t>dàolì</t>
+  </si>
+  <si>
+    <t>headstand</t>
+  </si>
+  <si>
+    <t>啤酒</t>
+  </si>
+  <si>
+    <t>píjiǔ</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>桶</t>
+  </si>
+  <si>
+    <t>tǒng</t>
+  </si>
+  <si>
+    <t>bucket, barrel</t>
+  </si>
+  <si>
+    <t>肩膀</t>
+  </si>
+  <si>
+    <t>jiānbǎng</t>
+  </si>
+  <si>
+    <t>shoulders</t>
+  </si>
+  <si>
+    <t>脱臼</t>
+  </si>
+  <si>
+    <t>tuōjiù</t>
+  </si>
+  <si>
+    <t>dislocate</t>
+  </si>
+  <si>
+    <t>育</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>金</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>汤</t>
+  </si>
+  <si>
+    <t>tāng</t>
+  </si>
+  <si>
+    <t>soup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">泡汤	</t>
+  </si>
+  <si>
+    <t>pàotāng</t>
+  </si>
+  <si>
+    <t>hotsprings, bathe</t>
+  </si>
+  <si>
+    <t>空翻</t>
+  </si>
+  <si>
+    <t>kōngfān</t>
+  </si>
+  <si>
+    <t>flip</t>
+  </si>
+  <si>
+    <t>懂</t>
+  </si>
+  <si>
+    <t>dǒng</t>
+  </si>
+  <si>
+    <t>understand</t>
+  </si>
+  <si>
+    <t>传奇</t>
+  </si>
+  <si>
+    <t>chuánqí</t>
+  </si>
+  <si>
+    <t>legend</t>
+  </si>
+  <si>
+    <t>节</t>
+  </si>
+  <si>
+    <t>holiday</t>
+  </si>
+  <si>
+    <t>圣诞</t>
+  </si>
+  <si>
+    <t>shèngdàn</t>
+  </si>
+  <si>
+    <t>Christmas</t>
+  </si>
+  <si>
+    <t>礼</t>
+  </si>
+  <si>
+    <t>present</t>
+  </si>
+  <si>
+    <t>辉煌</t>
+  </si>
+  <si>
+    <t>huīhuáng</t>
+  </si>
+  <si>
+    <t>brilliant</t>
+  </si>
+  <si>
+    <t>台</t>
+  </si>
+  <si>
+    <t>tái</t>
+  </si>
+  <si>
+    <t>tower, station</t>
+  </si>
+  <si>
+    <t>台湾</t>
+  </si>
+  <si>
+    <t>táiwān</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>台词</t>
+  </si>
+  <si>
+    <t>táicí</t>
+  </si>
+  <si>
+    <t>quotes</t>
+  </si>
+  <si>
+    <t>丢</t>
+  </si>
+  <si>
+    <t>diū</t>
+  </si>
+  <si>
+    <t>leave</t>
+  </si>
+  <si>
+    <t>角</t>
+  </si>
+  <si>
+    <t>jiǎo</t>
+  </si>
+  <si>
+    <t>angle, actor, etc</t>
+  </si>
+  <si>
+    <t>落</t>
+  </si>
+  <si>
+    <t>luò</t>
+  </si>
+  <si>
+    <t>角落</t>
+  </si>
+  <si>
+    <t>jiǎoluò</t>
+  </si>
+  <si>
+    <t>corner</t>
+  </si>
+  <si>
+    <t>身</t>
+  </si>
+  <si>
+    <t>shēn</t>
+  </si>
+  <si>
+    <t>停</t>
+  </si>
+  <si>
+    <t>tíng</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>停车</t>
+  </si>
+  <si>
+    <t>tíngchē</t>
+  </si>
+  <si>
+    <t>parking</t>
+  </si>
+  <si>
+    <t>声</t>
+  </si>
+  <si>
+    <t>shēng</t>
+  </si>
+  <si>
+    <t>voice</t>
+  </si>
+  <si>
+    <t>伪</t>
+  </si>
+  <si>
+    <t>wěi</t>
+  </si>
+  <si>
+    <t>psuedo, forget</t>
+  </si>
+  <si>
+    <t>伪装</t>
+  </si>
+  <si>
+    <t>wěizhuāng</t>
+  </si>
+  <si>
+    <t>disguise</t>
+  </si>
+  <si>
+    <t>衣装</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yīzhuāng	</t>
+  </si>
+  <si>
+    <t>clothes</t>
+  </si>
+  <si>
+    <t>尽</t>
+  </si>
+  <si>
+    <t>jǐn</t>
+  </si>
+  <si>
+    <t>all, exhaust</t>
+  </si>
+  <si>
+    <t>办法</t>
+  </si>
+  <si>
+    <t>bànfǎ</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>程</t>
+  </si>
+  <si>
+    <t>procedure, journey</t>
+  </si>
+  <si>
+    <t>老兄</t>
+  </si>
+  <si>
+    <t>lǎoxiōng</t>
+  </si>
+  <si>
+    <t>dude</t>
+  </si>
+  <si>
+    <t>贪婪</t>
+  </si>
+  <si>
+    <t>tānlán</t>
+  </si>
+  <si>
+    <t>greedy</t>
+  </si>
+  <si>
+    <t>处</t>
+  </si>
+  <si>
+    <t>chù</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>好处</t>
+  </si>
+  <si>
+    <t>hǎochù</t>
+  </si>
+  <si>
+    <t>benefit</t>
+  </si>
+  <si>
+    <t>欠</t>
+  </si>
+  <si>
+    <t>qiàn</t>
+  </si>
+  <si>
+    <t>owe</t>
+  </si>
+  <si>
+    <t>人情</t>
+  </si>
+  <si>
+    <t>rénqíng</t>
+  </si>
+  <si>
+    <t>favor</t>
+  </si>
+  <si>
+    <t>还清</t>
+  </si>
+  <si>
+    <t>huánqīng</t>
+  </si>
+  <si>
+    <t>pay off</t>
+  </si>
+  <si>
+    <t>满足</t>
+  </si>
+  <si>
+    <t>mǎnzú</t>
+  </si>
+  <si>
+    <t>satisfy</t>
+  </si>
+  <si>
+    <t>足</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>扯</t>
+  </si>
+  <si>
+    <t>chě</t>
+  </si>
+  <si>
+    <t>pull, gossip</t>
+  </si>
+  <si>
+    <t>平</t>
+  </si>
+  <si>
+    <t>flat</t>
+  </si>
+  <si>
+    <t>扯平</t>
+  </si>
+  <si>
+    <t>chěpíng</t>
+  </si>
+  <si>
+    <t>even</t>
+  </si>
+  <si>
+    <t>公平</t>
+  </si>
+  <si>
+    <t>gōngpíng</t>
+  </si>
+  <si>
+    <t>fair</t>
+  </si>
+  <si>
+    <t>捷径</t>
+  </si>
+  <si>
+    <t>jiéjìng</t>
+  </si>
+  <si>
+    <t>shortcut</t>
+  </si>
+  <si>
+    <t>预</t>
+  </si>
+  <si>
+    <t>pre</t>
+  </si>
+  <si>
+    <t>付款</t>
+  </si>
+  <si>
+    <t>fùkuǎn</t>
+  </si>
+  <si>
+    <t>payment</t>
+  </si>
+  <si>
+    <t>内</t>
+  </si>
+  <si>
+    <t>nèi</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>内置</t>
+  </si>
+  <si>
+    <t>nèizhì</t>
+  </si>
+  <si>
+    <t>built in</t>
+  </si>
+  <si>
+    <t>加热·</t>
+  </si>
+  <si>
+    <t>jiārè</t>
+  </si>
+  <si>
+    <t>heating</t>
+  </si>
+  <si>
+    <t>设备</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shèbèi	</t>
+  </si>
+  <si>
+    <t>真皮</t>
+  </si>
+  <si>
+    <t>zhēnpí</t>
+  </si>
+  <si>
+    <t>leather</t>
+  </si>
+  <si>
+    <t>座</t>
+  </si>
+  <si>
+    <t>zuò</t>
+  </si>
+  <si>
+    <t>seat</t>
+  </si>
+  <si>
+    <t>椅</t>
+  </si>
+  <si>
+    <t>yǐ</t>
+  </si>
+  <si>
+    <t>chair</t>
+  </si>
+  <si>
+    <t>痒</t>
+  </si>
+  <si>
+    <t>yǎng</t>
+  </si>
+  <si>
+    <t>itch</t>
+  </si>
+  <si>
+    <t>不痛不痒</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bùtòngbùyǎng	</t>
+  </si>
+  <si>
+    <t>superficial (harmless?)</t>
+  </si>
+  <si>
+    <t>唬</t>
+  </si>
+  <si>
+    <t>hǔ</t>
+  </si>
+  <si>
+    <t>fool, bluff</t>
+  </si>
+  <si>
+    <t>伎俩</t>
+  </si>
+  <si>
+    <t>jìliǎng</t>
+  </si>
+  <si>
+    <t>trick</t>
+  </si>
+  <si>
+    <t>殖民地</t>
+  </si>
+  <si>
+    <t>zhímíndì</t>
+  </si>
+  <si>
+    <t>colony</t>
+  </si>
+  <si>
+    <t>原因</t>
+  </si>
+  <si>
+    <t>yuányīn</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>佬</t>
+  </si>
+  <si>
+    <t>lǎo</t>
+  </si>
+  <si>
+    <t>guy</t>
+  </si>
+  <si>
+    <t>失</t>
+  </si>
+  <si>
+    <t>shī</t>
+  </si>
+  <si>
+    <t>取消</t>
+  </si>
+  <si>
+    <t>qǔxiāo</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>听证</t>
+  </si>
+  <si>
+    <t>tīngzhèng</t>
+  </si>
+  <si>
+    <t>hearing</t>
+  </si>
+  <si>
+    <t>愉</t>
+  </si>
+  <si>
+    <t>yú</t>
+  </si>
+  <si>
+    <t>delight</t>
+  </si>
+  <si>
+    <t>辆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liàng	</t>
+  </si>
+  <si>
+    <t>MW for vehicles</t>
+  </si>
+  <si>
+    <t>环</t>
+  </si>
+  <si>
+    <t>huán</t>
+  </si>
+  <si>
+    <t>ring</t>
+  </si>
+  <si>
+    <t>环保</t>
+  </si>
+  <si>
+    <t>huánbǎo</t>
+  </si>
+  <si>
+    <t>environmentally friendly</t>
+  </si>
+  <si>
+    <t>树叶</t>
+  </si>
+  <si>
+    <t>shùyè</t>
+  </si>
+  <si>
+    <t>leaves</t>
+  </si>
+  <si>
+    <t>擦</t>
+  </si>
+  <si>
+    <t>cā</t>
+  </si>
+  <si>
+    <t>wipe</t>
+  </si>
+  <si>
+    <t>屁股</t>
+  </si>
+  <si>
+    <t>pìgu</t>
+  </si>
+  <si>
+    <t>ass</t>
+  </si>
+  <si>
+    <t>烂</t>
+  </si>
+  <si>
+    <t>làn</t>
+  </si>
+  <si>
+    <t>高尔夫·</t>
+  </si>
+  <si>
+    <t>gāoěrfū</t>
+  </si>
+  <si>
+    <t>golf</t>
+  </si>
+  <si>
+    <t>里面</t>
+  </si>
+  <si>
+    <t>lǐmiàn</t>
+  </si>
+  <si>
+    <t>inside</t>
+  </si>
+  <si>
+    <t>泰</t>
+  </si>
+  <si>
+    <t>tài</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>料</t>
+  </si>
+  <si>
+    <t>liào</t>
+  </si>
+  <si>
+    <t>feed</t>
+  </si>
+  <si>
+    <t>料理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liàolǐ	</t>
+  </si>
+  <si>
+    <t>cuisine</t>
+  </si>
+  <si>
+    <t>计策</t>
+  </si>
+  <si>
+    <t>jìcè</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>煽动</t>
+  </si>
+  <si>
+    <t>shāndòng</t>
+  </si>
+  <si>
+    <t>incite</t>
+  </si>
+  <si>
+    <t>群</t>
+  </si>
+  <si>
+    <t>qún</t>
+  </si>
+  <si>
+    <t>昂</t>
+  </si>
+  <si>
+    <t>áng</t>
+  </si>
+  <si>
+    <t>high (elevation, not state)</t>
+  </si>
+  <si>
+    <t>激</t>
+  </si>
+  <si>
+    <t>stimulate, excite</t>
+  </si>
+  <si>
+    <t>乱成</t>
+  </si>
+  <si>
+    <t xml:space="preserve">luànchéng	</t>
+  </si>
+  <si>
+    <t>chaos</t>
+  </si>
+  <si>
+    <t>一片</t>
+  </si>
+  <si>
+    <t>yīpiàn</t>
+  </si>
+  <si>
+    <t>one piece</t>
+  </si>
+  <si>
+    <t>机会</t>
+  </si>
+  <si>
+    <t>jīhuì</t>
+  </si>
+  <si>
+    <t>chance</t>
+  </si>
+  <si>
+    <t>折</t>
+  </si>
+  <si>
+    <t>zhé</t>
+  </si>
+  <si>
+    <t>fold, break</t>
+  </si>
+  <si>
+    <t>折腾</t>
+  </si>
+  <si>
+    <t>zhéteng</t>
+  </si>
+  <si>
+    <t>toss</t>
+  </si>
+  <si>
+    <t>恭维</t>
+  </si>
+  <si>
+    <t>gōngwéi</t>
+  </si>
+  <si>
+    <t>compliment</t>
+  </si>
+  <si>
+    <t>荒谬</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huāngmiù	</t>
+  </si>
+  <si>
+    <t>absurd</t>
+  </si>
+  <si>
+    <t>至极</t>
+  </si>
+  <si>
+    <t>zhìjí</t>
+  </si>
+  <si>
+    <t>像样</t>
+  </si>
+  <si>
+    <t>xiàngyàng</t>
+  </si>
+  <si>
+    <t>decent</t>
+  </si>
+  <si>
+    <t>收拾</t>
+  </si>
+  <si>
+    <t>shōushí</t>
+  </si>
+  <si>
+    <t>clean</t>
+  </si>
+  <si>
+    <t>进</t>
+  </si>
+  <si>
+    <t>enter</t>
+  </si>
+  <si>
+    <t>烂摊</t>
+  </si>
+  <si>
+    <t>làntān</t>
+  </si>
+  <si>
+    <t>mess</t>
+  </si>
+  <si>
+    <t>屋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wū	</t>
+  </si>
+  <si>
+    <t>总统</t>
+  </si>
+  <si>
+    <t>zǒngtǒng</t>
+  </si>
+  <si>
+    <t>president</t>
+  </si>
+  <si>
+    <t>奥巴</t>
+  </si>
+  <si>
+    <t>àobā</t>
+  </si>
+  <si>
+    <t>Obama</t>
+  </si>
+  <si>
+    <t>搞定</t>
+  </si>
+  <si>
+    <t>gǎodìng</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>忘记</t>
+  </si>
+  <si>
+    <t>wàngjì</t>
+  </si>
+  <si>
+    <t>forget</t>
+  </si>
+  <si>
+    <t>肤</t>
+  </si>
+  <si>
+    <t>fū</t>
+  </si>
+  <si>
+    <t>skin</t>
+  </si>
+  <si>
+    <t>肤浅</t>
+  </si>
+  <si>
+    <t>fūqiǎn</t>
+  </si>
+  <si>
+    <t>shallow</t>
+  </si>
+  <si>
+    <t>渣</t>
+  </si>
+  <si>
+    <t>zhā</t>
+  </si>
+  <si>
+    <t>jag</t>
+  </si>
+  <si>
+    <t>乖（乖）</t>
+  </si>
+  <si>
+    <t>guāi</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>各</t>
+  </si>
+  <si>
+    <t>gè</t>
+  </si>
+  <si>
+    <t>each</t>
+  </si>
+  <si>
+    <t>各位</t>
+  </si>
+  <si>
+    <t>gèwèi</t>
+  </si>
+  <si>
+    <t>喊</t>
+  </si>
+  <si>
+    <t>hǎn</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>语气</t>
+  </si>
+  <si>
+    <t>yǔqì</t>
+  </si>
+  <si>
+    <t>tone</t>
+  </si>
+  <si>
+    <t>动物</t>
+  </si>
+  <si>
+    <t>dòngwù</t>
+  </si>
+  <si>
+    <t>animal</t>
+  </si>
+  <si>
+    <t>区别</t>
+  </si>
+  <si>
+    <t>qūbié</t>
+  </si>
+  <si>
+    <t>differene</t>
+  </si>
+  <si>
+    <t>脚</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jiǎo	</t>
+  </si>
+  <si>
+    <t>脚丫</t>
+  </si>
+  <si>
+    <t>jiǎoyā</t>
+  </si>
+  <si>
+    <t>feet</t>
+  </si>
+  <si>
+    <t>熊</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xióng	</t>
+  </si>
+  <si>
+    <t>bear</t>
+  </si>
+  <si>
+    <t>掌</t>
+  </si>
+  <si>
+    <t>zhǎng</t>
+  </si>
+  <si>
+    <t>palms</t>
+  </si>
+  <si>
+    <t>地球</t>
+  </si>
+  <si>
+    <t>dìqiú</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>观看</t>
+  </si>
+  <si>
+    <t>guānkàn</t>
+  </si>
+  <si>
+    <t>observe</t>
+  </si>
+  <si>
+    <t>探索</t>
+  </si>
+  <si>
+    <t>tànsuǒ</t>
+  </si>
+  <si>
+    <t>频道</t>
+  </si>
+  <si>
+    <t>píndào</t>
+  </si>
+  <si>
+    <t>channels</t>
+  </si>
+  <si>
+    <t>鲨鱼</t>
+  </si>
+  <si>
+    <t>shāyú</t>
+  </si>
+  <si>
+    <t>shark</t>
+  </si>
+  <si>
+    <t>同样</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tóngyàng	</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>支</t>
+  </si>
+  <si>
+    <t>zhī</t>
+  </si>
+  <si>
+    <t>MW for pens, branch</t>
+  </si>
+  <si>
+    <t>拿</t>
+  </si>
+  <si>
+    <t>ná</t>
+  </si>
+  <si>
+    <t>告诉</t>
+  </si>
+  <si>
+    <t>gàosù</t>
+  </si>
+  <si>
+    <t>深</t>
+  </si>
+  <si>
+    <t>deep</t>
+  </si>
+  <si>
+    <t>怜悯</t>
+  </si>
+  <si>
+    <t>liánmǐn</t>
+  </si>
+  <si>
+    <t>mercy</t>
+  </si>
+  <si>
+    <t>原谅</t>
+  </si>
+  <si>
+    <t>yuánliàng</t>
+  </si>
+  <si>
+    <t>forgive</t>
+  </si>
+  <si>
+    <t>佳</t>
+  </si>
+  <si>
+    <t>jiā</t>
+  </si>
+  <si>
+    <t>原创</t>
+  </si>
+  <si>
+    <t>yuánchuàng</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>剧</t>
+  </si>
+  <si>
+    <t>drama</t>
+  </si>
+  <si>
+    <t>剧本</t>
+  </si>
+  <si>
+    <t>jùběn</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>独</t>
+  </si>
+  <si>
+    <t>alone</t>
+  </si>
+  <si>
+    <t>长处</t>
+  </si>
+  <si>
+    <t>chángchu</t>
+  </si>
+  <si>
+    <t>advantages</t>
+  </si>
+  <si>
+    <t>对于</t>
+  </si>
+  <si>
+    <t>duìyú</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>明摆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">míngbǎi	</t>
+  </si>
+  <si>
+    <t>obvious, clearly</t>
+  </si>
+  <si>
+    <t>厉害</t>
+  </si>
+  <si>
+    <t>lìhài</t>
+  </si>
+  <si>
+    <t>awesome, sharp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chinese </t>
   </si>
   <si>
@@ -4499,12 +5804,6 @@
     <t>list, notice</t>
   </si>
   <si>
-    <t>拿</t>
-  </si>
-  <si>
-    <t>ná</t>
-  </si>
-  <si>
     <t>take</t>
   </si>
   <si>
@@ -4532,24 +5831,12 @@
     <t>static</t>
   </si>
   <si>
-    <t>脚</t>
-  </si>
-  <si>
-    <t>jiǎo</t>
-  </si>
-  <si>
-    <t>foot</t>
-  </si>
-  <si>
     <t>脚本</t>
   </si>
   <si>
     <t>jiǎoběn</t>
   </si>
   <si>
-    <t>script</t>
-  </si>
-  <si>
     <t>改</t>
   </si>
   <si>
@@ -4620,9 +5907,6 @@
   </si>
   <si>
     <t xml:space="preserve">fāngfǎ		</t>
-  </si>
-  <si>
-    <t>method</t>
   </si>
   <si>
     <t>不过</t>
@@ -10416,6 +11700,1711 @@
         <v>1450</v>
       </c>
     </row>
+    <row r="471">
+      <c r="A471" s="1" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B471" s="1" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C471" s="1" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B472" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C472" s="1" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="1" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B473" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C473" s="1" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B474" s="1" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C474" s="1" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="1" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C475" s="1" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="1" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B476" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C476" s="1" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C477" s="1" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C478" s="1" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C479" s="1" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="1" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B480" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C480" s="1" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B481" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C481" s="1" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="1" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B482" s="1" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C482" s="1" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C483" s="1" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="1" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C484" s="1" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="1" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C485" s="1" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C486" s="1" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="1" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B487" s="1" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C487" s="1" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C488" s="1" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B489" s="1" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C489" s="1" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="1" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C490" s="1" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="1" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C491" s="1" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="1" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C492" s="1" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="1" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C493" s="1" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C494" s="1" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="1" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C495" s="1" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C496" s="1" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="1" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C497" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="1" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C498" s="1" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C499" s="1" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="1" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C500" s="1" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="1" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C501" s="1" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="C502" s="1" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="1" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C503" s="1" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="C504" s="1" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C505" s="1" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="1" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C506" s="1" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C507" s="1" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C508" s="1" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C509" s="1" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C510" s="1" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C511" s="1" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="1" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C512" s="1" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="1" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C513" s="1" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="1" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C514" s="1" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="1" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C515" s="1" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="1" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C516" s="1" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C517" s="1" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="1" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C518" s="1" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="1" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C519" s="1" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="1" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>1590</v>
+      </c>
+      <c r="C520" s="1" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="1" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C521" s="1" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C522" s="1" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="1" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C523" s="1" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="1" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C524" s="1" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="1" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C525" s="1" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="1" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B526" s="1" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C526" s="1" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="1" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B527" s="1" t="s">
+        <v>1610</v>
+      </c>
+      <c r="C527" s="1" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="1" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C528" s="1" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="1" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B529" s="1" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C529" s="1" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="1" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C530" s="1" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="1" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C531" s="1" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="1" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B532" s="1" t="s">
+        <v>1624</v>
+      </c>
+      <c r="C532" s="1" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="1" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C533" s="1" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="1" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C534" s="1" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="1" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C535" s="1" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="1" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>1635</v>
+      </c>
+      <c r="C536" s="1" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="1" t="s">
+        <v>1637</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C537" s="1" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="C538" s="1" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="1" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C539" s="1" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="1" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>1646</v>
+      </c>
+      <c r="C540" s="1" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="1" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>1649</v>
+      </c>
+      <c r="C541" s="1" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="1" t="s">
+        <v>1651</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>1652</v>
+      </c>
+      <c r="C542" s="1" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="1" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C543" s="1" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="1" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>1657</v>
+      </c>
+      <c r="C544" s="1" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>1660</v>
+      </c>
+      <c r="C545" s="1" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="1" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B546" s="1" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C546" s="1" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="C547" s="1" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="1" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C548" s="1" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="1" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C549" s="1" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="1" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B550" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C550" s="1" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="1" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C551" s="1" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="1" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B552" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C552" s="1" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="1" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B553" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="C553" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B554" s="1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C554" s="1" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B555" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C555" s="1" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C556" s="1" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C557" s="1" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="1" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="1" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="1" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C560" s="1" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="1" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C561" s="1" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="1" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C562" s="1" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="1" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C563" s="1" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="1" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C564" s="1" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C565" s="1" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="1" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>1721</v>
+      </c>
+      <c r="C566" s="1" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="1" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C567" s="1" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="1" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C568" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="1" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C569" s="1" t="s">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="1" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C570" s="1" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="1" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C571" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="1" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C572" s="1" t="s">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="1" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B573" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C573" s="1" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="1" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B574" s="1" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C574" s="1" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B575" s="1" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C575" s="1" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B576" s="1" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C576" s="1" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="1" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B577" s="1" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C577" s="1" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="1" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B578" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C578" s="1" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="1" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B579" s="1" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C579" s="1" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C580" s="1" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B581" s="1" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C581" s="1" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" s="1" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B582" s="1" t="s">
+        <v>1766</v>
+      </c>
+      <c r="C582" s="1" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B583" s="1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C583" s="1" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B584" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C584" s="1" t="s">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="1" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B585" s="1" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C585" s="1" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B586" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C586" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B587" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C587" s="1" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B588" s="1" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C588" s="1" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B589" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C589" s="1" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" s="1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B590" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C590" s="1" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B591" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C591" s="1" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B592" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C592" s="1" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C593" s="1" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" s="1" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B594" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C594" s="1" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" s="1" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B595" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C595" s="1" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" s="1" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B596" s="1" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C596" s="1" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" s="1" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B597" s="1" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C597" s="1" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" s="1" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B598" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C598" s="1" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" s="1" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B599" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C599" s="1" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" s="1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B600" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="C600" s="1" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B601" s="1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C601" s="1" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B602" s="1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C602" s="1" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B603" s="1" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C603" s="1" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" s="1" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B604" s="1" t="s">
+        <v>1828</v>
+      </c>
+      <c r="C604" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B605" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C605" s="1" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" s="1" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B606" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C606" s="1" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B607" s="1" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C607" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B608" s="1" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C608" s="1" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B609" s="1" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C609" s="1" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" s="1" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B610" s="1" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C610" s="1" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" s="1" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B611" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C611" s="1" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" s="1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B612" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C612" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B613" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C613" s="1" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B614" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C614" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B615" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C615" s="1" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" s="1" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B616" s="1" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C616" s="1" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B617" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C617" s="1" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B618" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C618" s="1" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" s="1" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B619" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C619" s="1" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" s="1" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B620" s="1" t="s">
+        <v>1870</v>
+      </c>
+      <c r="C620" s="1" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" s="1" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B621" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="C621" s="1" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" s="1" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B622" s="1" t="s">
+        <v>1875</v>
+      </c>
+      <c r="C622" s="1" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" s="1" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B623" s="1" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C623" s="1" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" s="1" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B624" s="1" t="s">
+        <v>1881</v>
+      </c>
+      <c r="C624" s="1" t="s">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" s="1" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B625" s="1" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C625" s="1" t="s">
+        <v>1885</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -10433,16 +13422,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1451</v>
+        <v>1886</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1452</v>
+        <v>1887</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1453</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="2">
@@ -10453,195 +13442,195 @@
         <v>858</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1454</v>
+        <v>1889</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1455</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>1456</v>
+        <v>1891</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1457</v>
+        <v>1892</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1458</v>
+        <v>1893</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>1460</v>
+        <v>1895</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1461</v>
+        <v>1896</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1462</v>
+        <v>1897</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>1463</v>
+        <v>1898</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1464</v>
+        <v>1899</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1465</v>
+        <v>1900</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1455</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>1466</v>
+        <v>1901</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1467</v>
+        <v>1902</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1468</v>
+        <v>1903</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>1469</v>
+        <v>1904</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1470</v>
+        <v>1905</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1471</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>1472</v>
+        <v>1907</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1473</v>
+        <v>1908</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1474</v>
+        <v>1909</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>1475</v>
+        <v>1910</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1476</v>
+        <v>1911</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1477</v>
+        <v>1912</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>1478</v>
+        <v>1913</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1479</v>
+        <v>1914</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1480</v>
+        <v>1915</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>1481</v>
+        <v>1916</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1482</v>
+        <v>1917</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1483</v>
+        <v>1918</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1484</v>
+        <v>1919</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1485</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>1486</v>
+        <v>1921</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1487</v>
+        <v>1922</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1488</v>
+        <v>1923</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>1489</v>
+        <v>1924</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1490</v>
+        <v>1925</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1491</v>
+        <v>1926</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>1492</v>
+        <v>1927</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1493</v>
+        <v>1928</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1494</v>
+        <v>1929</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>1495</v>
+        <v>1850</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1496</v>
+        <v>1851</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1497</v>
+        <v>1930</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1498</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="16">
@@ -10652,38 +13641,38 @@
         <v>628</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1499</v>
+        <v>1932</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1455</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>1500</v>
+        <v>1933</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1501</v>
+        <v>1934</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1502</v>
+        <v>1935</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>1503</v>
+        <v>1936</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1504</v>
+        <v>1937</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1505</v>
+        <v>1938</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="19">
@@ -10697,49 +13686,49 @@
         <v>1344</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>1506</v>
+        <v>1819</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1507</v>
+        <v>1562</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1508</v>
+        <v>1622</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>1509</v>
+        <v>1939</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1510</v>
+        <v>1940</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1511</v>
+        <v>1871</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>1512</v>
+        <v>1941</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1513</v>
+        <v>1942</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1514</v>
+        <v>1943</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="23">
@@ -10753,35 +13742,35 @@
         <v>1000</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1455</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>1515</v>
+        <v>1944</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1516</v>
+        <v>1945</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1517</v>
+        <v>1946</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>1518</v>
+        <v>1947</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1519</v>
+        <v>1948</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1520</v>
+        <v>1949</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1455</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="26">
@@ -10789,122 +13778,122 @@
         <v>1177</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1521</v>
+        <v>1950</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>1179</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1455</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>1522</v>
+        <v>1951</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1523</v>
+        <v>1952</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1524</v>
+        <v>1953</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>1525</v>
+        <v>1954</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1526</v>
+        <v>1955</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1527</v>
+        <v>1956</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>1528</v>
+        <v>1957</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1529</v>
+        <v>1958</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1530</v>
+        <v>1959</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>1531</v>
+        <v>1960</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1532</v>
+        <v>1961</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1533</v>
+        <v>1962</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>1534</v>
+        <v>1963</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1535</v>
+        <v>1964</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1536</v>
+        <v>1594</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>1537</v>
+        <v>1965</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1538</v>
+        <v>1966</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1539</v>
+        <v>1967</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1540</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>1541</v>
+        <v>1969</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1542</v>
+        <v>1970</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1543</v>
+        <v>1971</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1459</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>1544</v>
+        <v>1972</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1545</v>
+        <v>1973</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1546</v>
+        <v>1974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>